<commit_message>
added total values to excel sheet
</commit_message>
<xml_diff>
--- a/measurementvalues.xlsx
+++ b/measurementvalues.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
   <si>
     <t>ENERGEST</t>
   </si>
@@ -53,6 +53,9 @@
   <si>
     <t>SECONDS</t>
   </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
 </sst>
 </file>
 
@@ -75,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -94,6 +97,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -107,11 +116,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -394,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,411 +855,501 @@
         <v>44.98016357421875</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <f>A5+A6+A7+A8+A9+A10+A11+A12+A13+A14</f>
+        <v>51149</v>
+      </c>
+      <c r="B15" s="4">
+        <f t="shared" ref="B15:F15" si="5">B5+B6+B7+B8+B9+B10+B11+B12+B13+B14</f>
+        <v>8868463</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" si="5"/>
+        <v>65</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="5"/>
+        <v>3190</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="5"/>
+        <v>7369036</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="4">
+        <f>G5+G6+G7+G8+G9+G10+G11+G12+G13+G14</f>
+        <v>1.560943603515625</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" ref="H15:K15" si="6">H5+H6+H7+H8+H9+H10+H11+H12+H13+H14</f>
+        <v>270.64401245117188</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="6"/>
+        <v>1.983642578125E-3</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="6"/>
+        <v>9.735107421875E-2</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" si="6"/>
+        <v>224.8851318359375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="K19" s="2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1570</v>
-      </c>
-      <c r="B19">
-        <v>153263</v>
-      </c>
-      <c r="C19">
-        <v>1003</v>
-      </c>
-      <c r="D19">
-        <v>267</v>
-      </c>
-      <c r="E19">
-        <v>280</v>
-      </c>
-      <c r="G19">
-        <f>A19/$D$1</f>
-        <v>4.791259765625E-2</v>
-      </c>
-      <c r="H19">
-        <f>B19/$D$1</f>
-        <v>4.677215576171875</v>
-      </c>
-      <c r="I19">
-        <f>C19/$D$1</f>
-        <v>3.0609130859375E-2</v>
-      </c>
-      <c r="J19">
-        <f>D19/$D$1</f>
-        <v>8.148193359375E-3</v>
-      </c>
-      <c r="K19">
-        <f>E19/$D$1</f>
-        <v>8.544921875E-3</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>3718</v>
+        <v>1570</v>
       </c>
       <c r="B20">
-        <v>314955</v>
+        <v>153263</v>
       </c>
       <c r="C20">
-        <v>1176</v>
+        <v>1003</v>
       </c>
       <c r="D20">
-        <v>534</v>
+        <v>267</v>
       </c>
       <c r="E20">
-        <v>163844</v>
+        <v>280</v>
       </c>
       <c r="G20">
-        <f t="shared" ref="G20:G28" si="5">A20/$D$1</f>
-        <v>0.11346435546875</v>
+        <f>A20/$D$1</f>
+        <v>4.791259765625E-2</v>
       </c>
       <c r="H20">
-        <f t="shared" ref="H20:H28" si="6">B20/$D$1</f>
-        <v>9.611663818359375</v>
+        <f>B20/$D$1</f>
+        <v>4.677215576171875</v>
       </c>
       <c r="I20">
-        <f t="shared" ref="I20:I28" si="7">C20/$D$1</f>
-        <v>3.5888671875E-2</v>
+        <f>C20/$D$1</f>
+        <v>3.0609130859375E-2</v>
       </c>
       <c r="J20">
-        <f t="shared" ref="J20:J28" si="8">D20/$D$1</f>
-        <v>1.629638671875E-2</v>
+        <f>D20/$D$1</f>
+        <v>8.148193359375E-3</v>
       </c>
       <c r="K20">
-        <f t="shared" ref="K20:K28" si="9">E20/$D$1</f>
-        <v>5.0001220703125</v>
+        <f>E20/$D$1</f>
+        <v>8.544921875E-3</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>5886</v>
+        <v>3718</v>
       </c>
       <c r="B21">
-        <v>476839</v>
+        <v>314955</v>
       </c>
       <c r="C21">
-        <v>1308</v>
+        <v>1176</v>
       </c>
       <c r="D21">
-        <v>801</v>
+        <v>534</v>
       </c>
       <c r="E21">
-        <v>327621</v>
+        <v>163844</v>
       </c>
       <c r="G21">
-        <f t="shared" si="5"/>
-        <v>0.17962646484375</v>
+        <f t="shared" ref="G21:G29" si="7">A21/$D$1</f>
+        <v>0.11346435546875</v>
       </c>
       <c r="H21">
-        <f t="shared" si="6"/>
-        <v>14.551971435546875</v>
+        <f t="shared" ref="H21:H29" si="8">B21/$D$1</f>
+        <v>9.611663818359375</v>
       </c>
       <c r="I21">
-        <f t="shared" si="7"/>
-        <v>3.99169921875E-2</v>
+        <f t="shared" ref="I21:I29" si="9">C21/$D$1</f>
+        <v>3.5888671875E-2</v>
       </c>
       <c r="J21">
-        <f t="shared" si="8"/>
-        <v>2.4444580078125E-2</v>
+        <f t="shared" ref="J21:J29" si="10">D21/$D$1</f>
+        <v>1.629638671875E-2</v>
       </c>
       <c r="K21">
-        <f t="shared" si="9"/>
-        <v>9.998199462890625</v>
+        <f t="shared" ref="K21:K29" si="11">E21/$D$1</f>
+        <v>5.0001220703125</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>7486</v>
+        <v>5886</v>
       </c>
       <c r="B22">
-        <v>638867</v>
+        <v>476839</v>
       </c>
       <c r="C22">
-        <v>1328</v>
+        <v>1308</v>
       </c>
       <c r="D22">
-        <v>1069</v>
+        <v>801</v>
       </c>
       <c r="E22">
-        <v>490973</v>
+        <v>327621</v>
       </c>
       <c r="G22">
-        <f t="shared" si="5"/>
-        <v>0.22845458984375</v>
+        <f t="shared" si="7"/>
+        <v>0.17962646484375</v>
       </c>
       <c r="H22">
-        <f t="shared" si="6"/>
-        <v>19.496673583984375</v>
+        <f t="shared" si="8"/>
+        <v>14.551971435546875</v>
       </c>
       <c r="I22">
-        <f t="shared" si="7"/>
-        <v>4.052734375E-2</v>
+        <f t="shared" si="9"/>
+        <v>3.99169921875E-2</v>
       </c>
       <c r="J22">
-        <f t="shared" si="8"/>
-        <v>3.2623291015625E-2</v>
+        <f t="shared" si="10"/>
+        <v>2.4444580078125E-2</v>
       </c>
       <c r="K22">
-        <f t="shared" si="9"/>
-        <v>14.983306884765625</v>
+        <f t="shared" si="11"/>
+        <v>9.998199462890625</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>9007</v>
+        <v>7486</v>
       </c>
       <c r="B23">
-        <v>801186</v>
+        <v>638867</v>
       </c>
       <c r="C23">
-        <v>1503</v>
+        <v>1328</v>
       </c>
       <c r="D23">
-        <v>1337</v>
+        <v>1069</v>
       </c>
       <c r="E23">
-        <v>654537</v>
+        <v>490973</v>
       </c>
       <c r="G23">
-        <f t="shared" si="5"/>
-        <v>0.274871826171875</v>
+        <f t="shared" si="7"/>
+        <v>0.22845458984375</v>
       </c>
       <c r="H23">
-        <f t="shared" si="6"/>
-        <v>24.45025634765625</v>
+        <f t="shared" si="8"/>
+        <v>19.496673583984375</v>
       </c>
       <c r="I23">
-        <f t="shared" si="7"/>
-        <v>4.5867919921875E-2</v>
+        <f t="shared" si="9"/>
+        <v>4.052734375E-2</v>
       </c>
       <c r="J23">
-        <f t="shared" si="8"/>
-        <v>4.0802001953125E-2</v>
+        <f t="shared" si="10"/>
+        <v>3.2623291015625E-2</v>
       </c>
       <c r="K23">
-        <f t="shared" si="9"/>
-        <v>19.974884033203125</v>
+        <f t="shared" si="11"/>
+        <v>14.983306884765625</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>10527</v>
+        <v>9007</v>
       </c>
       <c r="B24">
-        <v>963506</v>
+        <v>801186</v>
       </c>
       <c r="C24">
-        <v>1675</v>
+        <v>1503</v>
       </c>
       <c r="D24">
-        <v>1605</v>
+        <v>1337</v>
       </c>
       <c r="E24">
-        <v>818101</v>
+        <v>654537</v>
       </c>
       <c r="G24">
-        <f t="shared" si="5"/>
-        <v>0.321258544921875</v>
+        <f t="shared" si="7"/>
+        <v>0.274871826171875</v>
       </c>
       <c r="H24">
-        <f t="shared" si="6"/>
-        <v>29.40386962890625</v>
+        <f t="shared" si="8"/>
+        <v>24.45025634765625</v>
       </c>
       <c r="I24">
-        <f t="shared" si="7"/>
-        <v>5.1116943359375E-2</v>
+        <f t="shared" si="9"/>
+        <v>4.5867919921875E-2</v>
       </c>
       <c r="J24">
-        <f t="shared" si="8"/>
-        <v>4.8980712890625E-2</v>
+        <f t="shared" si="10"/>
+        <v>4.0802001953125E-2</v>
       </c>
       <c r="K24">
-        <f t="shared" si="9"/>
-        <v>24.966461181640625</v>
+        <f t="shared" si="11"/>
+        <v>19.974884033203125</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>12024</v>
+        <v>10527</v>
       </c>
       <c r="B25">
-        <v>1125849</v>
+        <v>963506</v>
       </c>
       <c r="C25">
         <v>1675</v>
       </c>
       <c r="D25">
-        <v>1873</v>
+        <v>1605</v>
       </c>
       <c r="E25">
-        <v>981655</v>
+        <v>818101</v>
       </c>
       <c r="G25">
-        <f t="shared" si="5"/>
-        <v>0.366943359375</v>
+        <f t="shared" si="7"/>
+        <v>0.321258544921875</v>
       </c>
       <c r="H25">
-        <f t="shared" si="6"/>
-        <v>34.358184814453125</v>
+        <f t="shared" si="8"/>
+        <v>29.40386962890625</v>
       </c>
       <c r="I25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5.1116943359375E-2</v>
       </c>
       <c r="J25">
-        <f t="shared" si="8"/>
-        <v>5.7159423828125E-2</v>
+        <f t="shared" si="10"/>
+        <v>4.8980712890625E-2</v>
       </c>
       <c r="K25">
-        <f t="shared" si="9"/>
-        <v>29.957733154296875</v>
+        <f t="shared" si="11"/>
+        <v>24.966461181640625</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>13524</v>
+        <v>12024</v>
       </c>
       <c r="B26">
-        <v>1288189</v>
+        <v>1125849</v>
       </c>
       <c r="C26">
-        <v>1869</v>
+        <v>1675</v>
       </c>
       <c r="D26">
-        <v>2141</v>
+        <v>1873</v>
       </c>
       <c r="E26">
-        <v>1145230</v>
+        <v>981655</v>
       </c>
       <c r="G26">
-        <f t="shared" si="5"/>
-        <v>0.4127197265625</v>
+        <f t="shared" si="7"/>
+        <v>0.366943359375</v>
       </c>
       <c r="H26">
-        <f t="shared" si="6"/>
-        <v>39.312408447265625</v>
+        <f t="shared" si="8"/>
+        <v>34.358184814453125</v>
       </c>
       <c r="I26">
-        <f t="shared" si="7"/>
-        <v>5.7037353515625E-2</v>
+        <f t="shared" si="9"/>
+        <v>5.1116943359375E-2</v>
       </c>
       <c r="J26">
-        <f t="shared" si="8"/>
-        <v>6.5338134765625E-2</v>
+        <f t="shared" si="10"/>
+        <v>5.7159423828125E-2</v>
       </c>
       <c r="K26">
-        <f t="shared" si="9"/>
-        <v>34.94964599609375</v>
+        <f t="shared" si="11"/>
+        <v>29.957733154296875</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>15026</v>
+        <v>13524</v>
       </c>
       <c r="B27">
-        <v>1450527</v>
+        <v>1288189</v>
       </c>
       <c r="C27">
-        <v>2506</v>
+        <v>1869</v>
       </c>
       <c r="D27">
-        <v>2408</v>
+        <v>2141</v>
       </c>
       <c r="E27">
-        <v>1308795</v>
+        <v>1145230</v>
       </c>
       <c r="G27">
-        <f t="shared" si="5"/>
-        <v>0.45855712890625</v>
+        <f t="shared" si="7"/>
+        <v>0.4127197265625</v>
       </c>
       <c r="H27">
-        <f t="shared" si="6"/>
-        <v>44.266571044921875</v>
+        <f t="shared" si="8"/>
+        <v>39.312408447265625</v>
       </c>
       <c r="I27">
-        <f t="shared" si="7"/>
-        <v>7.647705078125E-2</v>
+        <f t="shared" si="9"/>
+        <v>5.7037353515625E-2</v>
       </c>
       <c r="J27">
-        <f t="shared" si="8"/>
-        <v>7.3486328125E-2</v>
+        <f t="shared" si="10"/>
+        <v>6.5338134765625E-2</v>
       </c>
       <c r="K27">
-        <f t="shared" si="9"/>
-        <v>39.941253662109375</v>
+        <f t="shared" si="11"/>
+        <v>34.94964599609375</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
+        <v>15026</v>
+      </c>
+      <c r="B28">
+        <v>1450527</v>
+      </c>
+      <c r="C28">
+        <v>2506</v>
+      </c>
+      <c r="D28">
+        <v>2408</v>
+      </c>
+      <c r="E28">
+        <v>1308795</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="7"/>
+        <v>0.45855712890625</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="8"/>
+        <v>44.266571044921875</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="9"/>
+        <v>7.647705078125E-2</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="10"/>
+        <v>7.3486328125E-2</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="11"/>
+        <v>39.941253662109375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>16529</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>1612865</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>3143</v>
       </c>
-      <c r="D28">
+      <c r="D29">
         <v>2676</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <v>1472360</v>
       </c>
-      <c r="G28">
-        <f t="shared" si="5"/>
+      <c r="G29">
+        <f t="shared" si="7"/>
         <v>0.504425048828125</v>
       </c>
-      <c r="H28">
-        <f t="shared" si="6"/>
+      <c r="H29">
+        <f t="shared" si="8"/>
         <v>49.220733642578125</v>
       </c>
-      <c r="I28">
-        <f t="shared" si="7"/>
+      <c r="I29">
+        <f t="shared" si="9"/>
         <v>9.5916748046875E-2</v>
       </c>
-      <c r="J28">
-        <f t="shared" si="8"/>
+      <c r="J29">
+        <f t="shared" si="10"/>
         <v>8.16650390625E-2</v>
       </c>
-      <c r="K28">
-        <f t="shared" si="9"/>
+      <c r="K29">
+        <f t="shared" si="11"/>
         <v>44.932861328125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <f>A20+A21+A22+A23+A24+A25+A26+A27+A28+A29</f>
+        <v>95297</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" ref="B30:E30" si="12">B20+B21+B22+B23+B24+B25+B26+B27+B28+B29</f>
+        <v>8826046</v>
+      </c>
+      <c r="C30" s="4">
+        <f t="shared" si="12"/>
+        <v>17186</v>
+      </c>
+      <c r="D30" s="4">
+        <f t="shared" si="12"/>
+        <v>14711</v>
+      </c>
+      <c r="E30" s="4">
+        <f t="shared" si="12"/>
+        <v>7363396</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="4">
+        <f>G20+G21+G22+G23+G24+G25+G26+G27+G28+G29</f>
+        <v>2.908233642578125</v>
+      </c>
+      <c r="H30" s="4">
+        <f t="shared" ref="H30:K30" si="13">H20+H21+H22+H23+H24+H25+H26+H27+H28+H29</f>
+        <v>269.34954833984375</v>
+      </c>
+      <c r="I30" s="4">
+        <f t="shared" si="13"/>
+        <v>0.52447509765625</v>
+      </c>
+      <c r="J30" s="4">
+        <f t="shared" si="13"/>
+        <v>0.448944091796875</v>
+      </c>
+      <c r="K30" s="4">
+        <f t="shared" si="13"/>
+        <v>224.7130126953125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>